<commit_message>
Update the very baaad results
</commit_message>
<xml_diff>
--- a/Expereiments/OfflieClsutering.xlsx
+++ b/Expereiments/OfflieClsutering.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -140,13 +140,7 @@
     <t xml:space="preserve"> DBSCAN + Arabert</t>
   </si>
   <si>
-    <t>AraBert 512</t>
-  </si>
-  <si>
     <t xml:space="preserve">AraBert 768 </t>
-  </si>
-  <si>
-    <t>AraBert 256</t>
   </si>
   <si>
     <t>AraBert 128</t>
@@ -158,17 +152,74 @@
     <t>AraBert</t>
   </si>
   <si>
-    <t xml:space="preserve">SinglePass + ARabert </t>
+    <t>HDBSCAN + Arabert</t>
   </si>
   <si>
-    <t>HDBSCAN + Arabert</t>
+    <t>DBSCAN + Arabert + Named Entities</t>
+  </si>
+  <si>
+    <t>SinglePass +Arabert</t>
+  </si>
+  <si>
+    <t># Classes</t>
+  </si>
+  <si>
+    <t>Conherent (CV)</t>
+  </si>
+  <si>
+    <t>Coherent(Umass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DBSCAN + mBert</t>
+  </si>
+  <si>
+    <t>DBSCAN + mBert + Named Entities</t>
+  </si>
+  <si>
+    <t>HDBSCAN + mBert</t>
+  </si>
+  <si>
+    <t>SinglePass +mBert</t>
+  </si>
+  <si>
+    <t>AraBert 320</t>
+  </si>
+  <si>
+    <t>AraBert 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mBert 768 </t>
+  </si>
+  <si>
+    <t>mBert 512</t>
+  </si>
+  <si>
+    <t>mBert 256</t>
+  </si>
+  <si>
+    <t>mBert 128</t>
+  </si>
+  <si>
+    <t>mBert 64</t>
+  </si>
+  <si>
+    <t>mBert 32</t>
+  </si>
+  <si>
+    <t>mBert 320</t>
+  </si>
+  <si>
+    <t>Exp. 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +243,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -254,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -418,11 +484,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,17 +552,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,38 +573,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,40 +627,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -866,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:L18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -880,10 +1010,11 @@
     <col min="10" max="10" width="12.81640625" customWidth="1"/>
     <col min="11" max="11" width="15.453125" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="22.7265625" customWidth="1"/>
+    <col min="14" max="14" width="18.26953125" customWidth="1"/>
     <col min="15" max="15" width="14.26953125" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="19.90625" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -905,8 +1036,8 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
       <c r="U1" s="3"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
@@ -925,25 +1056,25 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
       <c r="U2" s="3"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -962,25 +1093,25 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
       <c r="U3" s="3"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -999,23 +1130,23 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
       <c r="U4" s="3"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -1037,30 +1168,30 @@
       <c r="D5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33" t="s">
+      <c r="E5" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="39" t="s">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="33" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="35"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
       <c r="U5" s="3"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
@@ -1079,39 +1210,35 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="41"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" s="54" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="N6" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="O6" s="39" t="s">
         <v>30</v>
       </c>
+      <c r="P6" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
       <c r="U6" s="3"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -1130,23 +1257,23 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="44"/>
       <c r="H7" s="45"/>
       <c r="I7" s="45"/>
       <c r="J7" s="46"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="3"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
@@ -1165,31 +1292,43 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="22" t="s">
+      <c r="E8" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="50"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="M8" s="67">
+        <v>0.17646800000000001</v>
+      </c>
+      <c r="N8" s="67">
+        <v>8.8158E-2</v>
+      </c>
+      <c r="O8" s="67">
+        <v>3.908E-3</v>
+      </c>
+      <c r="P8" s="67">
+        <v>120</v>
+      </c>
+      <c r="Q8" s="67">
+        <v>0.82015000000000005</v>
+      </c>
+      <c r="R8" s="67">
+        <v>-0.99522600000000006</v>
+      </c>
+      <c r="S8" s="66"/>
+      <c r="T8" s="66"/>
       <c r="U8" s="3"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -1208,25 +1347,37 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="49"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="22"/>
+      <c r="M9" s="68">
+        <v>0.198321</v>
+      </c>
+      <c r="N9" s="68">
+        <v>0.103009</v>
+      </c>
+      <c r="O9" s="68">
+        <v>4.64E-3</v>
+      </c>
+      <c r="P9" s="68">
+        <v>132</v>
+      </c>
+      <c r="Q9" s="68">
+        <v>0.81217499999999998</v>
+      </c>
+      <c r="R9" s="68">
+        <v>-1.0301290000000001</v>
+      </c>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
       <c r="U9" s="3"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
@@ -1245,25 +1396,37 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="58"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="67">
+        <v>0.22781699999999999</v>
+      </c>
+      <c r="N10" s="67">
+        <v>0.12594900000000001</v>
+      </c>
+      <c r="O10" s="67">
+        <v>5.8710000000000004E-3</v>
+      </c>
+      <c r="P10" s="67">
+        <v>143</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>0.79949400000000004</v>
+      </c>
+      <c r="R10" s="67">
+        <v>-1.047005</v>
+      </c>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
       <c r="U10" s="3"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
@@ -1282,25 +1445,37 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="56"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="36"/>
+      <c r="M11" s="70">
+        <v>0.27335300000000001</v>
+      </c>
+      <c r="N11" s="70">
+        <v>0.18811900000000001</v>
+      </c>
+      <c r="O11" s="70">
+        <v>1.042E-2</v>
+      </c>
+      <c r="P11" s="70">
+        <v>129</v>
+      </c>
+      <c r="Q11" s="70">
+        <v>0.82015000000000005</v>
+      </c>
+      <c r="R11" s="71">
+        <v>-0.99522600000000006</v>
+      </c>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
       <c r="U11" s="3"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
@@ -1319,27 +1494,27 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
       <c r="U12" s="3"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
@@ -1358,25 +1533,25 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="56"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
       <c r="U13" s="3"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
@@ -1395,25 +1570,25 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="58"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="67"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
       <c r="U14" s="3"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
@@ -1432,25 +1607,25 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="56"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="36"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
       <c r="U15" s="3"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
@@ -1469,27 +1644,27 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="58"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
       <c r="U16" s="3"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
@@ -1508,25 +1683,25 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" s="56"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="22"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
       <c r="U17" s="3"/>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
@@ -1545,25 +1720,25 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="58"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
       <c r="U18" s="3"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
@@ -1582,25 +1757,25 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="56"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="68"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
       <c r="U19" s="3"/>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
@@ -1619,31 +1794,27 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="50"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="23"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
       <c r="U20" s="3"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
@@ -1662,25 +1833,25 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="22"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
+      <c r="Q21" s="68"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
       <c r="U21" s="3"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
@@ -1699,25 +1870,25 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="50"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="34"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
       <c r="U22" s="3"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
@@ -1736,25 +1907,25 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" s="36"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
       <c r="U23" s="3"/>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
@@ -1773,27 +1944,43 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="50"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
+      <c r="D24" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="60"/>
+      <c r="G24" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" s="23"/>
+      <c r="M24" s="67">
+        <v>0.50558999999999998</v>
+      </c>
+      <c r="N24" s="67">
+        <v>0.415769</v>
+      </c>
+      <c r="O24" s="67">
+        <v>2.9503000000000001E-2</v>
+      </c>
+      <c r="P24" s="67">
+        <v>185</v>
+      </c>
+      <c r="Q24" s="67">
+        <v>0.694245</v>
+      </c>
+      <c r="R24" s="67">
+        <v>-1.2224219999999999</v>
+      </c>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
@@ -1812,25 +1999,37 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="49"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="22"/>
+      <c r="M25" s="68">
+        <v>0.506629</v>
+      </c>
+      <c r="N25" s="68">
+        <v>0.41648299999999999</v>
+      </c>
+      <c r="O25" s="68">
+        <v>2.9729999999999999E-2</v>
+      </c>
+      <c r="P25" s="68">
+        <v>187</v>
+      </c>
+      <c r="Q25" s="68">
+        <v>0.693747</v>
+      </c>
+      <c r="R25" s="68">
+        <v>-1.228872</v>
+      </c>
+      <c r="S25" s="66"/>
+      <c r="T25" s="66"/>
       <c r="U25" s="3"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
@@ -1849,25 +2048,37 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="50"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L26" s="23"/>
+      <c r="M26" s="74">
+        <v>0.50852399999999998</v>
+      </c>
+      <c r="N26" s="74">
+        <v>0.41818699999999998</v>
+      </c>
+      <c r="O26" s="74">
+        <v>3.0211999999999999E-2</v>
+      </c>
+      <c r="P26" s="74">
+        <v>189</v>
+      </c>
+      <c r="Q26" s="74">
+        <v>0.68921399999999999</v>
+      </c>
+      <c r="R26" s="74">
+        <v>-1.2351099999999999</v>
+      </c>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
       <c r="U26" s="3"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
@@ -1886,25 +2097,37 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="51"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L27" s="22"/>
+      <c r="M27" s="68">
+        <v>0.50597300000000001</v>
+      </c>
+      <c r="N27" s="68">
+        <v>0.42472799999999999</v>
+      </c>
+      <c r="O27" s="68">
+        <v>3.4550999999999998E-2</v>
+      </c>
+      <c r="P27" s="73">
+        <v>177</v>
+      </c>
+      <c r="Q27" s="73">
+        <v>0.68540100000000004</v>
+      </c>
+      <c r="R27" s="73">
+        <v>-1.2067749999999999</v>
+      </c>
+      <c r="S27" s="66"/>
+      <c r="T27" s="66"/>
       <c r="U27" s="3"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
@@ -1923,27 +2146,37 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="50"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="23"/>
+      <c r="M28" s="67">
+        <v>0.47901300000000002</v>
+      </c>
+      <c r="N28" s="67">
+        <v>0.42165399999999997</v>
+      </c>
+      <c r="O28" s="67">
+        <v>5.1840999999999998E-2</v>
+      </c>
+      <c r="P28" s="67">
+        <v>112</v>
+      </c>
+      <c r="Q28" s="67">
+        <v>0.66412099999999996</v>
+      </c>
+      <c r="R28" s="67">
+        <v>-0.96019399999999999</v>
+      </c>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
       <c r="U28" s="3"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
@@ -1962,25 +2195,37 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="L29" s="49"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L29" s="22"/>
+      <c r="M29" s="72">
+        <v>5.7762000000000001E-2</v>
+      </c>
+      <c r="N29" s="72">
+        <v>3.4737999999999998E-2</v>
+      </c>
+      <c r="O29" s="72">
+        <v>2.4550000000000002E-3</v>
+      </c>
+      <c r="P29" s="72">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="72">
+        <v>0.62182899999999997</v>
+      </c>
+      <c r="R29" s="72">
+        <v>-0.45506000000000002</v>
+      </c>
+      <c r="S29" s="66"/>
+      <c r="T29" s="66"/>
       <c r="U29" s="3"/>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
@@ -1999,25 +2244,27 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30" s="50"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" s="23"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
       <c r="U30" s="3"/>
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
@@ -2036,25 +2283,25 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="51"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" s="22"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="68"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="66"/>
       <c r="U31" s="3"/>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
@@ -2073,23 +2320,25 @@
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L32" s="23"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
       <c r="U32" s="3"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
@@ -2108,23 +2357,25 @@
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L33" s="22"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="66"/>
       <c r="U33" s="3"/>
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
@@ -2143,23 +2394,25 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L34" s="23"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
       <c r="U34" s="3"/>
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
@@ -2178,23 +2431,25 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="22"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="68"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="68"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
       <c r="U35" s="3"/>
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
@@ -2213,23 +2468,27 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
-      <c r="T36" s="17"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L36" s="23"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="67"/>
+      <c r="P36" s="67"/>
+      <c r="Q36" s="67"/>
+      <c r="R36" s="67"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
       <c r="U36" s="3"/>
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
@@ -2248,23 +2507,25 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L37" s="22"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="68"/>
+      <c r="P37" s="68"/>
+      <c r="Q37" s="68"/>
+      <c r="R37" s="68"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="3"/>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
@@ -2283,23 +2544,25 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L38" s="23"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="67"/>
+      <c r="P38" s="67"/>
+      <c r="Q38" s="67"/>
+      <c r="R38" s="67"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
       <c r="U38" s="3"/>
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
@@ -2318,23 +2581,25 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L39" s="22"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
       <c r="U39" s="3"/>
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
@@ -2353,23 +2618,25 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L40" s="23"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="67"/>
+      <c r="P40" s="67"/>
+      <c r="Q40" s="67"/>
+      <c r="R40" s="67"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
       <c r="U40" s="3"/>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
@@ -2388,23 +2655,27 @@
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="L41" s="22"/>
+      <c r="M41" s="68"/>
+      <c r="N41" s="68"/>
+      <c r="O41" s="68"/>
+      <c r="P41" s="68"/>
+      <c r="Q41" s="68"/>
+      <c r="R41" s="68"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
       <c r="U41" s="3"/>
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
@@ -2423,23 +2694,25 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L42" s="23"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="67"/>
+      <c r="Q42" s="67"/>
+      <c r="R42" s="67"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
       <c r="U42" s="3"/>
       <c r="V42" s="4"/>
       <c r="W42" s="4"/>
@@ -2458,23 +2731,25 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L43" s="22"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="68"/>
+      <c r="O43" s="68"/>
+      <c r="P43" s="68"/>
+      <c r="Q43" s="68"/>
+      <c r="R43" s="68"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
       <c r="U43" s="3"/>
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
@@ -2493,21 +2768,23 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" s="23"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="67"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="67"/>
+      <c r="Q44" s="67"/>
+      <c r="R44" s="67"/>
       <c r="S44" s="18"/>
       <c r="T44" s="18"/>
       <c r="U44" s="3"/>
@@ -2535,14 +2812,16 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
+      <c r="K45" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="L45" s="76"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="77"/>
+      <c r="P45" s="77"/>
+      <c r="Q45" s="77"/>
+      <c r="R45" s="77"/>
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
       <c r="U45" s="3"/>
@@ -2572,12 +2851,12 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
+      <c r="O46" s="67"/>
+      <c r="P46" s="67"/>
+      <c r="Q46" s="67"/>
+      <c r="R46" s="67"/>
       <c r="S46" s="18"/>
       <c r="T46" s="18"/>
       <c r="U46" s="3"/>
@@ -2607,12 +2886,12 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="69"/>
+      <c r="P47" s="69"/>
+      <c r="Q47" s="69"/>
+      <c r="R47" s="68"/>
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
       <c r="U47" s="3"/>
@@ -5136,35 +5415,43 @@
       <c r="AC128" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="E28:F31"/>
-    <mergeCell ref="G28:J31"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="D20:D31"/>
-    <mergeCell ref="E20:F23"/>
-    <mergeCell ref="G20:J23"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="E24:F27"/>
-    <mergeCell ref="G24:J27"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="G16:J19"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D8:D19"/>
-    <mergeCell ref="E8:F19"/>
+  <mergeCells count="66">
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="G41:J44"/>
+    <mergeCell ref="E24:F44"/>
+    <mergeCell ref="D24:D44"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="G24:J29"/>
+    <mergeCell ref="G30:J35"/>
+    <mergeCell ref="G36:J40"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="D3:R4"/>
+    <mergeCell ref="D2:R2"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:J7"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
     <mergeCell ref="G8:J11"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
@@ -5173,24 +5460,28 @@
     <mergeCell ref="G12:J15"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:J7"/>
-    <mergeCell ref="K6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="D2:T2"/>
-    <mergeCell ref="D3:T4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="E8:F23"/>
+    <mergeCell ref="D8:D23"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="G16:J19"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G20:J23"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5255,25 +5546,25 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
       <c r="U2" s="3"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -5292,25 +5583,25 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
       <c r="U3" s="3"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -5329,23 +5620,23 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
       <c r="U4" s="3"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -5367,30 +5658,30 @@
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="51"/>
+      <c r="G5" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="39" t="s">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="33" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="35"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="54"/>
       <c r="U5" s="3"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
@@ -5409,31 +5700,31 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="41"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="47" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="48"/>
-      <c r="O6" s="47" t="s">
+      <c r="N6" s="58"/>
+      <c r="O6" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="47" t="s">
+      <c r="P6" s="58"/>
+      <c r="Q6" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="48"/>
-      <c r="S6" s="47" t="s">
+      <c r="R6" s="58"/>
+      <c r="S6" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="48"/>
+      <c r="T6" s="58"/>
       <c r="U6" s="3"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -5452,15 +5743,15 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="44"/>
       <c r="H7" s="45"/>
       <c r="I7" s="45"/>
       <c r="J7" s="46"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
       <c r="M7" s="1" t="s">
         <v>5</v>
       </c>
@@ -5503,23 +5794,23 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="26"/>
+      <c r="G8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="50" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="50"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -5546,17 +5837,17 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="49" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="49"/>
+      <c r="L9" s="22"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -5583,17 +5874,17 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="50" t="s">
+      <c r="D10" s="32"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="50"/>
+      <c r="L10" s="23"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -5620,17 +5911,17 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="51" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="51"/>
+      <c r="L11" s="24"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -5657,17 +5948,17 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="50" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="50"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -5694,17 +5985,17 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="49" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="22"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -5731,17 +6022,17 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="50" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="50"/>
+      <c r="L14" s="23"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -5768,17 +6059,17 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="51" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="51"/>
+      <c r="L15" s="24"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
@@ -5805,17 +6096,17 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="50" t="s">
+      <c r="D16" s="32"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="50"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -5842,17 +6133,17 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="49" t="s">
+      <c r="D17" s="32"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="22"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -5879,17 +6170,17 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="50" t="s">
+      <c r="D18" s="32"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="50"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -5916,17 +6207,17 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="51" t="s">
+      <c r="D19" s="32"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="51"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -5953,23 +6244,23 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="22" t="s">
+      <c r="F20" s="26"/>
+      <c r="G20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="50" t="s">
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -5996,17 +6287,17 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="49" t="s">
+      <c r="D21" s="32"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="49"/>
+      <c r="L21" s="22"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -6033,17 +6324,17 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="50" t="s">
+      <c r="D22" s="32"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L22" s="50"/>
+      <c r="L22" s="23"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -6070,17 +6361,17 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="51" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L23" s="51"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -6107,19 +6398,19 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26" t="s">
+      <c r="D24" s="32"/>
+      <c r="E24" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="50" t="s">
+      <c r="F24" s="26"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="50"/>
+      <c r="L24" s="23"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -6146,17 +6437,17 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="49" t="s">
+      <c r="D25" s="32"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="49"/>
+      <c r="L25" s="22"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -6183,17 +6474,17 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="50" t="s">
+      <c r="D26" s="32"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="50"/>
+      <c r="L26" s="23"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
@@ -6220,17 +6511,17 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="51" t="s">
+      <c r="D27" s="32"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L27" s="51"/>
+      <c r="L27" s="24"/>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -6257,19 +6548,19 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="32"/>
+      <c r="E28" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="50" t="s">
+      <c r="F28" s="26"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="50"/>
+      <c r="L28" s="23"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -6296,17 +6587,17 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="49" t="s">
+      <c r="D29" s="32"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L29" s="49"/>
+      <c r="L29" s="22"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -6333,17 +6624,17 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="50" t="s">
+      <c r="D30" s="32"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L30" s="50"/>
+      <c r="L30" s="23"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -6370,17 +6661,17 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="51" t="s">
+      <c r="D31" s="32"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="51"/>
+      <c r="L31" s="24"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -9471,6 +9762,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="G16:J19"/>
+    <mergeCell ref="D8:D19"/>
+    <mergeCell ref="D20:D31"/>
+    <mergeCell ref="E20:F23"/>
+    <mergeCell ref="G20:J23"/>
+    <mergeCell ref="E24:F27"/>
+    <mergeCell ref="G24:J27"/>
+    <mergeCell ref="E28:F31"/>
+    <mergeCell ref="G28:J31"/>
+    <mergeCell ref="G8:J11"/>
+    <mergeCell ref="G12:J15"/>
+    <mergeCell ref="D2:T2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D3:T4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="G6:J7"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="E8:F19"/>
@@ -9487,40 +9812,6 @@
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="D2:T2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D3:T4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L7"/>
-    <mergeCell ref="G6:J7"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="G16:J19"/>
-    <mergeCell ref="D8:D19"/>
-    <mergeCell ref="D20:D31"/>
-    <mergeCell ref="E20:F23"/>
-    <mergeCell ref="G20:J23"/>
-    <mergeCell ref="E24:F27"/>
-    <mergeCell ref="G24:J27"/>
-    <mergeCell ref="E28:F31"/>
-    <mergeCell ref="G28:J31"/>
-    <mergeCell ref="G8:J11"/>
-    <mergeCell ref="G12:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9590,25 +9881,25 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
       <c r="U2" s="3"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -9627,25 +9918,25 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
       <c r="U3" s="3"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -9664,23 +9955,23 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
       <c r="U4" s="3"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -9702,30 +9993,30 @@
       <c r="D5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="51"/>
+      <c r="G5" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="39" t="s">
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="33" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="35"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="54"/>
       <c r="U5" s="3"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
@@ -9744,37 +10035,37 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="41"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
       <c r="J6" s="43"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="54" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="O6" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="54" t="s">
+      <c r="P6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="54" t="s">
+      <c r="Q6" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="R6" s="54" t="s">
+      <c r="R6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="S6" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="T6" s="39" t="s">
         <v>30</v>
       </c>
       <c r="U6" s="3"/>
@@ -9795,23 +10086,23 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="44"/>
       <c r="H7" s="45"/>
       <c r="I7" s="45"/>
       <c r="J7" s="46"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
       <c r="U7" s="3"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
@@ -9830,23 +10121,23 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="26"/>
+      <c r="G8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="50" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="50"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -9873,17 +10164,17 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="49" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="49"/>
+      <c r="L9" s="22"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -9910,17 +10201,17 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="50" t="s">
+      <c r="D10" s="32"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="50"/>
+      <c r="L10" s="23"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -9947,17 +10238,17 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="55" t="s">
+      <c r="D11" s="32"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="56"/>
+      <c r="L11" s="36"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -9984,17 +10275,17 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="50" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="L12" s="50"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -10021,17 +10312,17 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="49" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="22"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -10058,17 +10349,17 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="50" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="50"/>
+      <c r="L14" s="23"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -10095,17 +10386,17 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="55" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="56"/>
+      <c r="L15" s="36"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
@@ -10132,17 +10423,17 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="50" t="s">
+      <c r="D16" s="32"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="50"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -10169,17 +10460,17 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="49" t="s">
+      <c r="D17" s="32"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="22"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -10206,17 +10497,17 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="50" t="s">
+      <c r="D18" s="32"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L18" s="50"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -10243,17 +10534,17 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="55" t="s">
+      <c r="D19" s="32"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="56"/>
+      <c r="L19" s="36"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -10280,23 +10571,23 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="22" t="s">
+      <c r="F20" s="26"/>
+      <c r="G20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="50" t="s">
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -10323,17 +10614,17 @@
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="49" t="s">
+      <c r="D21" s="32"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="49"/>
+      <c r="L21" s="22"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -10360,17 +10651,17 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="50" t="s">
+      <c r="D22" s="32"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L22" s="50"/>
+      <c r="L22" s="23"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -10397,17 +10688,17 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="51" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L23" s="51"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -10434,19 +10725,19 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26" t="s">
+      <c r="D24" s="32"/>
+      <c r="E24" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="50" t="s">
+      <c r="F24" s="26"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="50"/>
+      <c r="L24" s="23"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -10473,17 +10764,17 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="49" t="s">
+      <c r="D25" s="32"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="49"/>
+      <c r="L25" s="22"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -10510,17 +10801,17 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="50" t="s">
+      <c r="D26" s="32"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="50"/>
+      <c r="L26" s="23"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
@@ -10547,17 +10838,17 @@
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="51" t="s">
+      <c r="D27" s="32"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L27" s="51"/>
+      <c r="L27" s="24"/>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -10584,19 +10875,19 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="32"/>
+      <c r="E28" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="50" t="s">
+      <c r="F28" s="26"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="50"/>
+      <c r="L28" s="23"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -10623,17 +10914,17 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="49" t="s">
+      <c r="D29" s="32"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L29" s="49"/>
+      <c r="L29" s="22"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -10660,17 +10951,17 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="50" t="s">
+      <c r="D30" s="32"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L30" s="50"/>
+      <c r="L30" s="23"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -10697,17 +10988,17 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="51" t="s">
+      <c r="D31" s="32"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="51"/>
+      <c r="L31" s="24"/>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -13798,39 +14089,11 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="D2:T2"/>
-    <mergeCell ref="D3:T4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="G6:J7"/>
-    <mergeCell ref="K6:L7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D8:D19"/>
-    <mergeCell ref="E8:F19"/>
-    <mergeCell ref="G8:J11"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="G12:J15"/>
-    <mergeCell ref="D20:D31"/>
-    <mergeCell ref="E20:F23"/>
-    <mergeCell ref="G20:J23"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="E24:F27"/>
-    <mergeCell ref="G24:J27"/>
-    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="P6:P7"/>
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K26:L26"/>
@@ -13847,11 +14110,39 @@
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="G16:J19"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="D20:D31"/>
+    <mergeCell ref="E20:F23"/>
+    <mergeCell ref="G20:J23"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="E24:F27"/>
+    <mergeCell ref="G24:J27"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="D8:D19"/>
+    <mergeCell ref="E8:F19"/>
+    <mergeCell ref="G8:J11"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="G12:J15"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="G6:J7"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="D2:T2"/>
+    <mergeCell ref="D3:T4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>